<commit_message>
Final Version After Push On Orch And Befor Clean Code
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\RPAMaterial\reframworkexamples\udemyRE\UdemyPerformer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E9B5564-9795-49F4-A263-154A07D28723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F27EF6B8-487C-4778-8836-3FB873CC3408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20415" windowHeight="10920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1775,7 +1775,7 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>24</v>

</xml_diff>